<commit_message>
Updated database URI after migrating to Supabase; Updated employees table fields
</commit_message>
<xml_diff>
--- a/Employees.xlsx
+++ b/Employees.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\TBCBackOffice\flask-backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync-Work\TBCBackOffice\flask-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264CD6D9-8A31-46AC-BA34-1E79488FFD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2830F29E-CE70-48D7-8F88-FADB1E0695A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9245CEF5-74EF-48D1-A8B7-253E393F9420}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="24792" windowHeight="14856" xr2:uid="{9245CEF5-74EF-48D1-A8B7-253E393F9420}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -59,15 +57,9 @@
     <t>email</t>
   </si>
   <si>
-    <t>hire_date</t>
-  </si>
-  <si>
     <t>end_date</t>
   </si>
   <si>
-    <t>active</t>
-  </si>
-  <si>
     <t>position</t>
   </si>
   <si>
@@ -203,9 +195,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>10992 Scarlet St, Loma Linda, 92354</t>
-  </si>
-  <si>
     <t>Brandon</t>
   </si>
   <si>
@@ -249,6 +238,27 @@
   </si>
   <si>
     <t>Both</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>Axel</t>
+  </si>
+  <si>
+    <t>Hui</t>
+  </si>
+  <si>
+    <t>Thammanit</t>
+  </si>
+  <si>
+    <t>Sawangchad</t>
+  </si>
+  <si>
+    <t>25581 Nikcs Avenue, Loma Linda, 92354</t>
   </si>
 </sst>
 </file>
@@ -638,26 +648,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE807097-07A9-4E0D-822D-92CF786C5858}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -668,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -686,19 +697,19 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -706,34 +717,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="I2" s="2">
         <v>45383</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -741,34 +752,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I3" s="2">
         <v>45383</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M3" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -776,16 +787,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
       </c>
       <c r="I4" s="2">
         <v>45352</v>
@@ -794,10 +805,10 @@
         <v>45868</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -805,19 +816,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2">
         <v>44927</v>
@@ -826,13 +837,13 @@
         <v>45747</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -840,31 +851,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I6" s="2">
         <v>45231</v>
       </c>
       <c r="K6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -872,19 +883,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I7" s="2">
         <v>45323</v>
@@ -893,13 +904,13 @@
         <v>45747</v>
       </c>
       <c r="K7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -907,28 +918,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I8" s="2">
         <v>42795</v>
       </c>
       <c r="K8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -936,28 +947,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I9" s="2">
         <v>42795</v>
       </c>
       <c r="K9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -965,28 +976,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I10" s="2">
         <v>42795</v>
       </c>
       <c r="K10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -994,19 +1005,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I11" s="2">
         <v>44927</v>
@@ -1015,13 +1026,13 @@
         <v>45747</v>
       </c>
       <c r="K11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1029,31 +1040,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I12" s="2">
         <v>42795</v>
       </c>
       <c r="K12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1061,28 +1072,86 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I13" s="2">
         <v>45597</v>
       </c>
       <c r="K13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M13" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="2">
+        <v>44866</v>
+      </c>
+      <c r="J14" s="2">
+        <v>45291</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="2">
+        <v>45397</v>
+      </c>
+      <c r="J15" s="2">
+        <v>45504</v>
+      </c>
+      <c r="K15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" t="s">
+        <v>64</v>
+      </c>
+      <c r="M15" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>